<commit_message>
Added stock price data from yfinance and datetime objects for all dataframes
</commit_message>
<xml_diff>
--- a/Financial Modelling Prep Library/Company Financial Data/AAPL/annual/balance_sheets.xlsx
+++ b/Financial Modelling Prep Library/Company Financial Data/AAPL/annual/balance_sheets.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="262">
   <si>
     <t>date</t>
   </si>
@@ -295,6 +295,15 @@
     <t>AAPL-FY-2022</t>
   </si>
   <si>
+    <t>AAPL</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>0000320193</t>
+  </si>
+  <si>
     <t>1985-09-30</t>
   </si>
   <si>
@@ -322,112 +331,19 @@
     <t>1993-09-30</t>
   </si>
   <si>
-    <t>1994-09-30</t>
-  </si>
-  <si>
-    <t>1995-09-29</t>
-  </si>
-  <si>
-    <t>1996-09-27</t>
-  </si>
-  <si>
-    <t>1997-09-26</t>
+    <t>1994-12-13</t>
+  </si>
+  <si>
+    <t>1995-12-19</t>
+  </si>
+  <si>
+    <t>1996-12-19</t>
+  </si>
+  <si>
+    <t>1997-12-05</t>
   </si>
   <si>
     <t>1998-09-25</t>
-  </si>
-  <si>
-    <t>1999-09-25</t>
-  </si>
-  <si>
-    <t>2000-09-30</t>
-  </si>
-  <si>
-    <t>2001-09-29</t>
-  </si>
-  <si>
-    <t>2002-09-28</t>
-  </si>
-  <si>
-    <t>2003-09-27</t>
-  </si>
-  <si>
-    <t>2004-09-25</t>
-  </si>
-  <si>
-    <t>2005-09-24</t>
-  </si>
-  <si>
-    <t>2006-09-30</t>
-  </si>
-  <si>
-    <t>2007-09-29</t>
-  </si>
-  <si>
-    <t>2008-09-27</t>
-  </si>
-  <si>
-    <t>2009-09-26</t>
-  </si>
-  <si>
-    <t>2010-09-25</t>
-  </si>
-  <si>
-    <t>2011-09-24</t>
-  </si>
-  <si>
-    <t>2012-09-29</t>
-  </si>
-  <si>
-    <t>2013-09-28</t>
-  </si>
-  <si>
-    <t>2014-09-27</t>
-  </si>
-  <si>
-    <t>2015-09-26</t>
-  </si>
-  <si>
-    <t>2016-09-24</t>
-  </si>
-  <si>
-    <t>2017-09-30</t>
-  </si>
-  <si>
-    <t>2018-09-29</t>
-  </si>
-  <si>
-    <t>2019-09-28</t>
-  </si>
-  <si>
-    <t>2020-09-26</t>
-  </si>
-  <si>
-    <t>2021-09-25</t>
-  </si>
-  <si>
-    <t>2022-09-24</t>
-  </si>
-  <si>
-    <t>AAPL</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>0000320193</t>
-  </si>
-  <si>
-    <t>1994-12-13</t>
-  </si>
-  <si>
-    <t>1995-12-19</t>
-  </si>
-  <si>
-    <t>1996-12-19</t>
-  </si>
-  <si>
-    <t>1997-12-05</t>
   </si>
   <si>
     <t>1999-12-22</t>
@@ -890,6 +806,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -953,11 +872,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1431,29 +1351,29 @@
       <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2">
+        <v>31320</v>
+      </c>
+      <c r="C2" t="s">
         <v>93</v>
       </c>
-      <c r="C2" t="s">
-        <v>131</v>
-      </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="H2" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="I2" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J2">
         <v>337000000</v>
@@ -1592,29 +1512,29 @@
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2">
+        <v>31685</v>
+      </c>
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" t="s">
         <v>94</v>
       </c>
-      <c r="C3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" t="s">
-        <v>132</v>
-      </c>
       <c r="E3" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G3" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
       <c r="H3" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
       <c r="I3" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J3">
         <v>576200000</v>
@@ -1753,29 +1673,29 @@
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2">
+        <v>32050</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" t="s">
         <v>95</v>
       </c>
-      <c r="C4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" t="s">
-        <v>133</v>
-      </c>
       <c r="F4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="H4" t="s">
-        <v>202</v>
+        <v>174</v>
       </c>
       <c r="I4" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J4">
         <v>565100000</v>
@@ -1914,29 +1834,29 @@
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B5" t="s">
-        <v>96</v>
+      <c r="B5" s="2">
+        <v>32416</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G5" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="H5" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="I5" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J5">
         <v>545700000</v>
@@ -2075,29 +1995,29 @@
       <c r="A6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B6" t="s">
-        <v>97</v>
+      <c r="B6" s="2">
+        <v>32781</v>
       </c>
       <c r="C6" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E6" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="H6" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
       <c r="I6" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J6">
         <v>438300000</v>
@@ -2236,29 +2156,29 @@
       <c r="A7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B7" t="s">
-        <v>98</v>
+      <c r="B7" s="2">
+        <v>33146</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E7" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G7" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="H7" t="s">
-        <v>205</v>
+        <v>177</v>
       </c>
       <c r="I7" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J7">
         <v>374700000</v>
@@ -2397,29 +2317,29 @@
       <c r="A8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B8" t="s">
-        <v>99</v>
+      <c r="B8" s="2">
+        <v>33511</v>
       </c>
       <c r="C8" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E8" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G8" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="H8" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
       <c r="I8" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J8">
         <v>604100000</v>
@@ -2558,29 +2478,29 @@
       <c r="A9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B9" t="s">
-        <v>100</v>
+      <c r="B9" s="2">
+        <v>33877</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E9" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G9" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="H9" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
       <c r="I9" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J9">
         <v>498600000</v>
@@ -2719,29 +2639,29 @@
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B10" t="s">
-        <v>101</v>
+      <c r="B10" s="2">
+        <v>34242</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F10" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G10" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="H10" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="I10" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J10">
         <v>676400000</v>
@@ -2880,29 +2800,29 @@
       <c r="A11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B11" t="s">
-        <v>102</v>
+      <c r="B11" s="2">
+        <v>34607</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E11" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F11" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="G11" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="H11" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
       <c r="I11" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J11">
         <v>1203488000</v>
@@ -3036,40 +2956,40 @@
       <c r="BA11">
         <v>-607288000</v>
       </c>
-      <c r="BB11" s="2" t="s">
+      <c r="BB11" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="BC11" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="BC11" s="2" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:55">
       <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B12" t="s">
-        <v>103</v>
+      <c r="B12" s="2">
+        <v>34971</v>
       </c>
       <c r="C12" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E12" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F12" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="G12" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="H12" t="s">
+        <v>182</v>
+      </c>
+      <c r="I12" t="s">
         <v>210</v>
-      </c>
-      <c r="I12" t="s">
-        <v>238</v>
       </c>
       <c r="J12">
         <v>756000000</v>
@@ -3203,40 +3123,40 @@
       <c r="BA12">
         <v>8000000</v>
       </c>
-      <c r="BB12" s="2" t="s">
+      <c r="BB12" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="BC12" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="BC12" s="2" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:55">
       <c r="A13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B13" t="s">
-        <v>104</v>
+      <c r="B13" s="2">
+        <v>35335</v>
       </c>
       <c r="C13" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F13" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="G13" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="H13" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="I13" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J13">
         <v>1552000000</v>
@@ -3370,40 +3290,40 @@
       <c r="BA13">
         <v>-417000000</v>
       </c>
-      <c r="BB13" s="2" t="s">
+      <c r="BB13" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="BC13" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="BC13" s="2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:55">
       <c r="A14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B14" t="s">
-        <v>105</v>
+      <c r="B14" s="2">
+        <v>35699</v>
       </c>
       <c r="C14" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E14" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F14" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="G14" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="H14" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="I14" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J14">
         <v>1230000000</v>
@@ -3537,40 +3457,40 @@
       <c r="BA14">
         <v>-254000000</v>
       </c>
-      <c r="BB14" s="2" t="s">
+      <c r="BB14" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="BC14" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="BC14" s="2" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:55">
       <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B15" t="s">
-        <v>106</v>
+      <c r="B15" s="2">
+        <v>36063</v>
       </c>
       <c r="C15" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E15" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G15" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="H15" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="I15" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J15">
         <v>1481000000</v>
@@ -3709,29 +3629,29 @@
       <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B16" t="s">
-        <v>107</v>
+      <c r="B16" s="2">
+        <v>36428</v>
       </c>
       <c r="C16" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D16" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E16" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F16" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="G16" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="H16" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="I16" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J16">
         <v>1326000000</v>
@@ -3865,40 +3785,40 @@
       <c r="BA16">
         <v>-1026000000</v>
       </c>
-      <c r="BB16" s="2" t="s">
+      <c r="BB16" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="BC16" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="BC16" s="2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:55">
       <c r="A17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B17" t="s">
-        <v>108</v>
+      <c r="B17" s="2">
+        <v>36799</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D17" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E17" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F17" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="G17" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
       <c r="H17" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="I17" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J17">
         <v>1191000000</v>
@@ -4032,40 +3952,40 @@
       <c r="BA17">
         <v>-891000000</v>
       </c>
-      <c r="BB17" s="2" t="s">
+      <c r="BB17" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="BC17" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="BC17" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:55">
       <c r="A18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B18" t="s">
-        <v>109</v>
+      <c r="B18" s="2">
+        <v>37163</v>
       </c>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E18" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F18" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="G18" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="H18" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="I18" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J18">
         <v>2310000000</v>
@@ -4199,40 +4119,40 @@
       <c r="BA18">
         <v>-1993000000</v>
       </c>
-      <c r="BB18" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="BC18" s="2" t="s">
-        <v>245</v>
+      <c r="BB18" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BC18" s="3" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:55">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B19" t="s">
-        <v>110</v>
+      <c r="B19" s="2">
+        <v>37527</v>
       </c>
       <c r="C19" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E19" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F19" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="G19" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="H19" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="I19" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J19">
         <v>2252000000</v>
@@ -4366,40 +4286,40 @@
       <c r="BA19">
         <v>-1936000000</v>
       </c>
-      <c r="BB19" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="BC19" s="2" t="s">
-        <v>273</v>
+      <c r="BB19" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="BC19" s="3" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:55">
       <c r="A20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B20" t="s">
-        <v>111</v>
+      <c r="B20" s="2">
+        <v>37891</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E20" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F20" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="G20" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="H20" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="I20" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J20">
         <v>3396000000</v>
@@ -4533,40 +4453,40 @@
       <c r="BA20">
         <v>-3092000000</v>
       </c>
-      <c r="BB20" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="BC20" s="2" t="s">
-        <v>247</v>
+      <c r="BB20" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="BC20" s="3" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:55">
       <c r="A21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B21" t="s">
-        <v>112</v>
+      <c r="B21" s="2">
+        <v>38255</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E21" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F21" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="G21" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="H21" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="I21" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J21">
         <v>2969000000</v>
@@ -4700,40 +4620,40 @@
       <c r="BA21">
         <v>-2969000000</v>
       </c>
-      <c r="BB21" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="BC21" s="2" t="s">
-        <v>248</v>
+      <c r="BB21" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="BC21" s="3" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:55">
       <c r="A22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B22" t="s">
-        <v>113</v>
+      <c r="B22" s="2">
+        <v>38619</v>
       </c>
       <c r="C22" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E22" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F22" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="G22" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="H22" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="I22" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J22">
         <v>3491000000</v>
@@ -4867,40 +4787,40 @@
       <c r="BA22">
         <v>-3491000000</v>
       </c>
-      <c r="BB22" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="BC22" s="2" t="s">
-        <v>249</v>
+      <c r="BB22" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="BC22" s="3" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:55">
       <c r="A23" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B23" t="s">
-        <v>114</v>
+      <c r="B23" s="2">
+        <v>38990</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F23" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="G23" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="H23" t="s">
-        <v>221</v>
+        <v>193</v>
       </c>
       <c r="I23" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J23">
         <v>6392000000</v>
@@ -5034,40 +4954,40 @@
       <c r="BA23">
         <v>-6392000000</v>
       </c>
-      <c r="BB23" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="BC23" s="2" t="s">
-        <v>250</v>
+      <c r="BB23" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="BC23" s="3" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:55">
       <c r="A24" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B24" t="s">
-        <v>115</v>
+      <c r="B24" s="2">
+        <v>39354</v>
       </c>
       <c r="C24" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E24" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F24" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="G24" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="H24" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
       <c r="I24" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J24">
         <v>9352000000</v>
@@ -5201,40 +5121,40 @@
       <c r="BA24">
         <v>-9352000000</v>
       </c>
-      <c r="BB24" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="BC24" s="2" t="s">
-        <v>274</v>
+      <c r="BB24" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="BC24" s="3" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:55">
       <c r="A25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B25" t="s">
-        <v>116</v>
+      <c r="B25" s="2">
+        <v>39718</v>
       </c>
       <c r="C25" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E25" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F25" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="G25" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
       <c r="H25" t="s">
-        <v>223</v>
+        <v>195</v>
       </c>
       <c r="I25" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J25">
         <v>11875000000</v>
@@ -5368,40 +5288,40 @@
       <c r="BA25">
         <v>-11875000000</v>
       </c>
-      <c r="BB25" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="BC25" s="2" t="s">
-        <v>275</v>
+      <c r="BB25" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="BC25" s="3" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:55">
       <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B26" t="s">
-        <v>117</v>
+      <c r="B26" s="2">
+        <v>40082</v>
       </c>
       <c r="C26" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E26" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F26" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="G26" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="H26" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
       <c r="I26" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J26">
         <v>5263000000</v>
@@ -5535,40 +5455,40 @@
       <c r="BA26">
         <v>-5263000000</v>
       </c>
-      <c r="BB26" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="BC26" s="2" t="s">
-        <v>276</v>
+      <c r="BB26" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="BC26" s="3" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="27" spans="1:55">
       <c r="A27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B27" t="s">
-        <v>118</v>
+      <c r="B27" s="2">
+        <v>40446</v>
       </c>
       <c r="C27" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E27" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F27" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="G27" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="H27" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="I27" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J27">
         <v>11261000000</v>
@@ -5702,40 +5622,40 @@
       <c r="BA27">
         <v>-11261000000</v>
       </c>
-      <c r="BB27" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="BC27" s="2" t="s">
-        <v>277</v>
+      <c r="BB27" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="BC27" s="3" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:55">
       <c r="A28" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B28" t="s">
-        <v>119</v>
+      <c r="B28" s="2">
+        <v>40810</v>
       </c>
       <c r="C28" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D28" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E28" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F28" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="G28" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="H28" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
       <c r="I28" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J28">
         <v>9815000000</v>
@@ -5869,40 +5789,40 @@
       <c r="BA28">
         <v>-9815000000</v>
       </c>
-      <c r="BB28" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="BC28" s="2" t="s">
-        <v>278</v>
+      <c r="BB28" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="BC28" s="3" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="29" spans="1:55">
       <c r="A29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B29" t="s">
-        <v>120</v>
+      <c r="B29" s="2">
+        <v>41181</v>
       </c>
       <c r="C29" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D29" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E29" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F29" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G29" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="H29" t="s">
-        <v>227</v>
+        <v>199</v>
       </c>
       <c r="I29" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J29">
         <v>10746000000</v>
@@ -6036,40 +5956,40 @@
       <c r="BA29">
         <v>-10746000000</v>
       </c>
-      <c r="BB29" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="BC29" s="2" t="s">
-        <v>279</v>
+      <c r="BB29" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="BC29" s="3" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:55">
       <c r="A30" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B30" t="s">
-        <v>121</v>
+      <c r="B30" s="2">
+        <v>41545</v>
       </c>
       <c r="C30" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D30" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E30" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F30" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="G30" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="H30" t="s">
-        <v>228</v>
+        <v>200</v>
       </c>
       <c r="I30" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J30">
         <v>14259000000</v>
@@ -6203,40 +6123,40 @@
       <c r="BA30">
         <v>2701000000</v>
       </c>
-      <c r="BB30" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="BC30" s="2" t="s">
-        <v>280</v>
+      <c r="BB30" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="BC30" s="3" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:55">
       <c r="A31" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B31" t="s">
-        <v>122</v>
+      <c r="B31" s="2">
+        <v>41909</v>
       </c>
       <c r="C31" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D31" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E31" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F31" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="G31" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="H31" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
       <c r="I31" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J31">
         <v>13844000000</v>
@@ -6370,40 +6290,40 @@
       <c r="BA31">
         <v>21451000000</v>
       </c>
-      <c r="BB31" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="BC31" s="2" t="s">
-        <v>281</v>
+      <c r="BB31" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="BC31" s="3" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="32" spans="1:55">
       <c r="A32" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B32" t="s">
-        <v>123</v>
+      <c r="B32" s="2">
+        <v>42273</v>
       </c>
       <c r="C32" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E32" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F32" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="G32" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="H32" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
       <c r="I32" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J32">
         <v>21120000000</v>
@@ -6537,40 +6457,40 @@
       <c r="BA32">
         <v>43342000000</v>
       </c>
-      <c r="BB32" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="BC32" s="2" t="s">
-        <v>282</v>
+      <c r="BB32" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="BC32" s="3" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="33" spans="1:55">
       <c r="A33" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B33" t="s">
-        <v>124</v>
+      <c r="B33" s="2">
+        <v>42637</v>
       </c>
       <c r="C33" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E33" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F33" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="G33" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="H33" t="s">
-        <v>231</v>
+        <v>203</v>
       </c>
       <c r="I33" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J33">
         <v>20484000000</v>
@@ -6704,40 +6624,40 @@
       <c r="BA33">
         <v>66548000000</v>
       </c>
-      <c r="BB33" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="BC33" s="2" t="s">
-        <v>283</v>
+      <c r="BB33" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="BC33" s="3" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="34" spans="1:55">
       <c r="A34" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B34" t="s">
-        <v>125</v>
+      <c r="B34" s="2">
+        <v>43008</v>
       </c>
       <c r="C34" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E34" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F34" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="G34" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="H34" t="s">
-        <v>232</v>
+        <v>204</v>
       </c>
       <c r="I34" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J34">
         <v>20289000000</v>
@@ -6871,40 +6791,40 @@
       <c r="BA34">
         <v>95391000000</v>
       </c>
-      <c r="BB34" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="BC34" s="2" t="s">
-        <v>284</v>
+      <c r="BB34" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="BC34" s="3" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="35" spans="1:55">
       <c r="A35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B35" t="s">
-        <v>126</v>
+      <c r="B35" s="2">
+        <v>43372</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D35" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E35" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F35" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="G35" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="H35" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="I35" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J35">
         <v>25913000000</v>
@@ -7038,40 +6958,40 @@
       <c r="BA35">
         <v>88570000000</v>
       </c>
-      <c r="BB35" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="BC35" s="2" t="s">
-        <v>285</v>
+      <c r="BB35" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="BC35" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="36" spans="1:55">
       <c r="A36" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B36" t="s">
-        <v>127</v>
+      <c r="B36" s="2">
+        <v>43736</v>
       </c>
       <c r="C36" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E36" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F36" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="G36" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="H36" t="s">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="I36" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J36">
         <v>48844000000</v>
@@ -7205,40 +7125,40 @@
       <c r="BA36">
         <v>59203000000</v>
       </c>
-      <c r="BB36" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="BC36" s="2" t="s">
-        <v>286</v>
+      <c r="BB36" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="BC36" s="3" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="1:55">
       <c r="A37" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B37" t="s">
-        <v>128</v>
+      <c r="B37" s="2">
+        <v>44100</v>
       </c>
       <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F37" t="s">
         <v>131</v>
       </c>
-      <c r="D37" t="s">
-        <v>132</v>
-      </c>
-      <c r="E37" t="s">
-        <v>133</v>
-      </c>
-      <c r="F37" t="s">
-        <v>159</v>
-      </c>
       <c r="G37" t="s">
-        <v>197</v>
+        <v>169</v>
       </c>
       <c r="H37" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
       <c r="I37" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J37">
         <v>38016000000</v>
@@ -7372,40 +7292,40 @@
       <c r="BA37">
         <v>74420000000</v>
       </c>
-      <c r="BB37" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="BC37" s="2" t="s">
-        <v>287</v>
+      <c r="BB37" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="BC37" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:55">
       <c r="A38" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B38" t="s">
-        <v>129</v>
+      <c r="B38" s="2">
+        <v>44464</v>
       </c>
       <c r="C38" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D38" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38" t="s">
         <v>132</v>
       </c>
-      <c r="E38" t="s">
-        <v>133</v>
-      </c>
-      <c r="F38" t="s">
-        <v>160</v>
-      </c>
       <c r="G38" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="H38" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="I38" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J38">
         <v>34940000000</v>
@@ -7539,40 +7459,40 @@
       <c r="BA38">
         <v>89779000000</v>
       </c>
-      <c r="BB38" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="BC38" s="2" t="s">
-        <v>288</v>
+      <c r="BB38" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="BC38" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:55">
       <c r="A39" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B39" t="s">
-        <v>130</v>
+      <c r="B39" s="2">
+        <v>44828</v>
       </c>
       <c r="C39" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D39" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="E39" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39" t="s">
         <v>133</v>
       </c>
-      <c r="F39" t="s">
-        <v>161</v>
-      </c>
       <c r="G39" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="H39" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
       <c r="I39" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="J39">
         <v>23646000000</v>
@@ -7706,11 +7626,11 @@
       <c r="BA39">
         <v>96423000000</v>
       </c>
-      <c r="BB39" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="BC39" s="2" t="s">
-        <v>289</v>
+      <c r="BB39" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="BC39" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>